<commit_message>
Final Commit before Submission
</commit_message>
<xml_diff>
--- a/ExperimentList.xlsx
+++ b/ExperimentList.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://herts365-my.sharepoint.com/personal/bt22aak_herts_ac_uk/Documents/ProjectWorkables/MscProjectRepo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="8_{8FB7EE8C-03D5-490C-A022-36A164B0F0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{975075B2-F89E-4354-A173-3511990EEEE7}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="8_{8FB7EE8C-03D5-490C-A022-36A164B0F0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C1644EB-2B43-4BDF-844C-135854DA1F06}"/>
   <bookViews>
-    <workbookView xWindow="16371" yWindow="0" windowWidth="16629" windowHeight="17880" xr2:uid="{373AC7B1-6464-4577-8099-CCADA7A31CED}"/>
+    <workbookView xWindow="69" yWindow="17" windowWidth="16388" windowHeight="8726" activeTab="2" xr2:uid="{373AC7B1-6464-4577-8099-CCADA7A31CED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -111,7 +113,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,13 +122,27 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <name val="Aptos Narrow"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,8 +155,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5B9BD5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBDD6EE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDEEAF6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -148,13 +182,111 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -173,6 +305,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -494,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B813C3E1-A61A-440A-8F3C-00DD70075391}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -555,7 +691,7 @@
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A9" s="2">
+      <c r="A9" s="10">
         <v>2</v>
       </c>
       <c r="B9" t="s">
@@ -563,44 +699,44 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A10" s="2"/>
+      <c r="A10" s="10"/>
       <c r="B10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A11" s="2"/>
+      <c r="A11" s="10"/>
       <c r="B11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A12" s="2"/>
+      <c r="A12" s="10"/>
       <c r="B12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A13" s="2"/>
+      <c r="A13" s="10"/>
       <c r="B13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A14" s="2"/>
+      <c r="A14" s="10"/>
       <c r="B14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A15" s="2"/>
+      <c r="A15" s="10"/>
       <c r="B15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
     <row r="17" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A17" s="2">
+      <c r="A17" s="10">
         <v>3</v>
       </c>
       <c r="B17" t="s">
@@ -608,25 +744,25 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A18" s="2"/>
+      <c r="A18" s="10"/>
       <c r="B18" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A19" s="2"/>
+      <c r="A19" s="10"/>
       <c r="B19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A20" s="2"/>
+      <c r="A20" s="10"/>
       <c r="B20" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A21" s="2"/>
+      <c r="A21" s="10"/>
       <c r="B21" t="s">
         <v>9</v>
       </c>
@@ -636,8 +772,677 @@
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A9:A15"/>
   </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899C534D-69F2-47D1-81EA-D9F01F9B96D0}">
+  <dimension ref="A1:U28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23:I28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="2">
+        <v>1883</v>
+      </c>
+      <c r="B1" s="3">
+        <v>57580</v>
+      </c>
+      <c r="C1" s="3">
+        <v>3136</v>
+      </c>
+      <c r="D1" s="4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="5">
+        <v>1891</v>
+      </c>
+      <c r="B2" s="6">
+        <v>58026</v>
+      </c>
+      <c r="C2" s="6">
+        <v>2690</v>
+      </c>
+      <c r="D2" s="6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="5">
+        <v>1890</v>
+      </c>
+      <c r="B3" s="7">
+        <v>57952</v>
+      </c>
+      <c r="C3" s="7">
+        <v>2764</v>
+      </c>
+      <c r="D3" s="7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="5">
+        <v>1888</v>
+      </c>
+      <c r="B4" s="6">
+        <v>57735</v>
+      </c>
+      <c r="C4" s="6">
+        <v>2981</v>
+      </c>
+      <c r="D4" s="6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="8">
+        <v>1900</v>
+      </c>
+      <c r="B5" s="7">
+        <v>57635</v>
+      </c>
+      <c r="C5" s="7">
+        <v>3081</v>
+      </c>
+      <c r="D5" s="7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="G6" s="2">
+        <v>1883</v>
+      </c>
+      <c r="H6" s="5">
+        <v>1891</v>
+      </c>
+      <c r="I6" s="5">
+        <v>1890</v>
+      </c>
+      <c r="J6" s="5">
+        <v>1888</v>
+      </c>
+      <c r="K6" s="8">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="G7" s="3">
+        <v>57580</v>
+      </c>
+      <c r="H7" s="6">
+        <v>58026</v>
+      </c>
+      <c r="I7" s="7">
+        <v>57952</v>
+      </c>
+      <c r="J7" s="6">
+        <v>57735</v>
+      </c>
+      <c r="K7" s="7">
+        <v>57635</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="G8" s="3">
+        <v>3136</v>
+      </c>
+      <c r="H8" s="6">
+        <v>2690</v>
+      </c>
+      <c r="I8" s="7">
+        <v>2764</v>
+      </c>
+      <c r="J8" s="6">
+        <v>2981</v>
+      </c>
+      <c r="K8" s="7">
+        <v>3081</v>
+      </c>
+      <c r="P8" s="9">
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>0.35639999999999999</v>
+      </c>
+      <c r="R8" s="3">
+        <v>0.98850000000000005</v>
+      </c>
+      <c r="S8" s="3">
+        <v>0.94369999999999998</v>
+      </c>
+      <c r="T8" s="3">
+        <v>0.52929999999999999</v>
+      </c>
+      <c r="U8" s="4">
+        <v>0.57720000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="G9" s="4">
+        <v>33</v>
+      </c>
+      <c r="H9" s="6">
+        <v>25</v>
+      </c>
+      <c r="I9" s="7">
+        <v>26</v>
+      </c>
+      <c r="J9" s="6">
+        <v>28</v>
+      </c>
+      <c r="K9" s="7">
+        <v>16</v>
+      </c>
+      <c r="P9" s="5">
+        <v>0.91539999999999999</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>0.26290000000000002</v>
+      </c>
+      <c r="R9" s="6">
+        <v>0.97809999999999997</v>
+      </c>
+      <c r="S9" s="6">
+        <v>0.91349999999999998</v>
+      </c>
+      <c r="T9" s="6">
+        <v>0.41439999999999999</v>
+      </c>
+      <c r="U9" s="6">
+        <v>0.93569999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="P10" s="5">
+        <v>0.95430000000000004</v>
+      </c>
+      <c r="Q10" s="7">
+        <v>0.39989999999999998</v>
+      </c>
+      <c r="R10" s="7">
+        <v>0.98540000000000005</v>
+      </c>
+      <c r="S10" s="7">
+        <v>0.95330000000000004</v>
+      </c>
+      <c r="T10" s="7">
+        <v>0.56889999999999996</v>
+      </c>
+      <c r="U10" s="7">
+        <v>0.48370000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="P11" s="5">
+        <v>0.94589999999999996</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>0.36</v>
+      </c>
+      <c r="R11" s="6">
+        <v>0.98880000000000001</v>
+      </c>
+      <c r="S11" s="6">
+        <v>0.9446</v>
+      </c>
+      <c r="T11" s="6">
+        <v>0.52769999999999995</v>
+      </c>
+      <c r="U11" s="6">
+        <v>0.61580000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="P12" s="5">
+        <v>0.94320000000000004</v>
+      </c>
+      <c r="Q12" s="7">
+        <v>0.34849999999999998</v>
+      </c>
+      <c r="R12" s="7">
+        <v>0.98429999999999995</v>
+      </c>
+      <c r="S12" s="7">
+        <v>0.94189999999999996</v>
+      </c>
+      <c r="T12" s="7">
+        <v>0.51470000000000005</v>
+      </c>
+      <c r="U12" s="7">
+        <v>0.84870000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="P13" s="8">
+        <v>0.94189999999999996</v>
+      </c>
+      <c r="Q13" s="6">
+        <v>0.3427</v>
+      </c>
+      <c r="R13" s="6">
+        <v>0.98119999999999996</v>
+      </c>
+      <c r="S13" s="6">
+        <v>0.94059999999999999</v>
+      </c>
+      <c r="T13" s="6">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="U13" s="6">
+        <v>0.63270000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C14" s="9">
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0.91539999999999999</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0.95430000000000004</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0.94589999999999996</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0.94320000000000004</v>
+      </c>
+      <c r="H14" s="8">
+        <v>0.94189999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C15" s="3">
+        <v>0.35639999999999999</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0.26290000000000002</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0.39989999999999998</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0.36</v>
+      </c>
+      <c r="G15" s="7">
+        <v>0.34849999999999998</v>
+      </c>
+      <c r="H15" s="6">
+        <v>0.3427</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C16" s="3">
+        <v>0.98850000000000005</v>
+      </c>
+      <c r="D16" s="6">
+        <v>0.97809999999999997</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0.98540000000000005</v>
+      </c>
+      <c r="F16" s="6">
+        <v>0.98880000000000001</v>
+      </c>
+      <c r="G16" s="7">
+        <v>0.98429999999999995</v>
+      </c>
+      <c r="H16" s="6">
+        <v>0.98119999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C17" s="3">
+        <v>0.94369999999999998</v>
+      </c>
+      <c r="D17" s="6">
+        <v>0.91349999999999998</v>
+      </c>
+      <c r="E17" s="7">
+        <v>0.95330000000000004</v>
+      </c>
+      <c r="F17" s="6">
+        <v>0.9446</v>
+      </c>
+      <c r="G17" s="7">
+        <v>0.94189999999999996</v>
+      </c>
+      <c r="H17" s="6">
+        <v>0.94059999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C18" s="3">
+        <v>0.52929999999999999</v>
+      </c>
+      <c r="D18" s="6">
+        <v>0.41439999999999999</v>
+      </c>
+      <c r="E18" s="7">
+        <v>0.56889999999999996</v>
+      </c>
+      <c r="F18" s="6">
+        <v>0.52769999999999995</v>
+      </c>
+      <c r="G18" s="7">
+        <v>0.51470000000000005</v>
+      </c>
+      <c r="H18" s="6">
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C19" s="4">
+        <v>0.57720000000000005</v>
+      </c>
+      <c r="D19" s="6">
+        <v>0.93569999999999998</v>
+      </c>
+      <c r="E19" s="7">
+        <v>0.48370000000000002</v>
+      </c>
+      <c r="F19" s="6">
+        <v>0.61580000000000001</v>
+      </c>
+      <c r="G19" s="7">
+        <v>0.84870000000000001</v>
+      </c>
+      <c r="H19" s="6">
+        <v>0.63270000000000004</v>
+      </c>
+      <c r="L19" s="9">
+        <v>0.94269999999999998</v>
+      </c>
+      <c r="M19" s="3">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="N19" s="3">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="O19" s="3">
+        <v>0.94130000000000003</v>
+      </c>
+      <c r="P19" s="3">
+        <v>0.51380000000000003</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>0.52300000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="L20" s="5">
+        <v>0.95089999999999997</v>
+      </c>
+      <c r="M20" s="6">
+        <v>0.38290000000000002</v>
+      </c>
+      <c r="N20" s="6">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="O20" s="6">
+        <v>0.94969999999999999</v>
+      </c>
+      <c r="P20" s="6">
+        <v>0.55210000000000004</v>
+      </c>
+      <c r="Q20" s="6">
+        <v>0.55559999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="L21" s="5">
+        <v>0.94769999999999999</v>
+      </c>
+      <c r="M21" s="7">
+        <v>0.36759999999999998</v>
+      </c>
+      <c r="N21" s="7">
+        <v>0.9849</v>
+      </c>
+      <c r="O21" s="7">
+        <v>0.94650000000000001</v>
+      </c>
+      <c r="P21" s="7">
+        <v>0.53539999999999999</v>
+      </c>
+      <c r="Q21" s="7">
+        <v>0.56889999999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="L22" s="5">
+        <v>0.95420000000000005</v>
+      </c>
+      <c r="M22" s="6">
+        <v>0.39939999999999998</v>
+      </c>
+      <c r="N22" s="6">
+        <v>0.98640000000000005</v>
+      </c>
+      <c r="O22" s="6">
+        <v>0.95320000000000005</v>
+      </c>
+      <c r="P22" s="6">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="Q22" s="6">
+        <v>0.5514</v>
+      </c>
+    </row>
+    <row r="23" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C23" s="9">
+        <v>0.94269999999999998</v>
+      </c>
+      <c r="D23" s="5">
+        <v>0.95089999999999997</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0.94769999999999999</v>
+      </c>
+      <c r="F23" s="5">
+        <v>0.95420000000000005</v>
+      </c>
+      <c r="G23" s="5">
+        <v>0.94440000000000002</v>
+      </c>
+      <c r="H23" s="5">
+        <v>0.93810000000000004</v>
+      </c>
+      <c r="I23" s="8">
+        <v>0.94589999999999996</v>
+      </c>
+      <c r="L23" s="5">
+        <v>0.94440000000000002</v>
+      </c>
+      <c r="M23" s="7">
+        <v>0.35399000000000003</v>
+      </c>
+      <c r="N23" s="7">
+        <v>0.99009999999999998</v>
+      </c>
+      <c r="O23" s="7">
+        <v>0.94289999999999996</v>
+      </c>
+      <c r="P23" s="7">
+        <v>0.52139999999999997</v>
+      </c>
+      <c r="Q23" s="7">
+        <v>0.53520000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C24" s="3">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0.38290000000000002</v>
+      </c>
+      <c r="E24" s="7">
+        <v>0.36759999999999998</v>
+      </c>
+      <c r="F24" s="6">
+        <v>0.39939999999999998</v>
+      </c>
+      <c r="G24" s="7">
+        <v>0.35399000000000003</v>
+      </c>
+      <c r="H24" s="6">
+        <v>0.32969999999999999</v>
+      </c>
+      <c r="I24" s="7">
+        <v>0.3599</v>
+      </c>
+      <c r="L24" s="5">
+        <v>0.93810000000000004</v>
+      </c>
+      <c r="M24" s="6">
+        <v>0.32969999999999999</v>
+      </c>
+      <c r="N24" s="6">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="O24" s="6">
+        <v>0.9365</v>
+      </c>
+      <c r="P24" s="6">
+        <v>0.4945</v>
+      </c>
+      <c r="Q24" s="6">
+        <v>0.60750000000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C25" s="3">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="E25" s="7">
+        <v>0.9849</v>
+      </c>
+      <c r="F25" s="6">
+        <v>0.98640000000000005</v>
+      </c>
+      <c r="G25" s="7">
+        <v>0.99009999999999998</v>
+      </c>
+      <c r="H25" s="6">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="I25" s="7">
+        <v>0.98640000000000005</v>
+      </c>
+      <c r="L25" s="8">
+        <v>0.94589999999999996</v>
+      </c>
+      <c r="M25" s="7">
+        <v>0.3599</v>
+      </c>
+      <c r="N25" s="7">
+        <v>0.98640000000000005</v>
+      </c>
+      <c r="O25" s="7">
+        <v>0.9446</v>
+      </c>
+      <c r="P25" s="7">
+        <v>0.52729999999999999</v>
+      </c>
+      <c r="Q25" s="7">
+        <v>0.58620000000000005</v>
+      </c>
+    </row>
+    <row r="26" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C26" s="3">
+        <v>0.94130000000000003</v>
+      </c>
+      <c r="D26" s="6">
+        <v>0.94969999999999999</v>
+      </c>
+      <c r="E26" s="7">
+        <v>0.94650000000000001</v>
+      </c>
+      <c r="F26" s="6">
+        <v>0.95320000000000005</v>
+      </c>
+      <c r="G26" s="7">
+        <v>0.94289999999999996</v>
+      </c>
+      <c r="H26" s="6">
+        <v>0.9365</v>
+      </c>
+      <c r="I26" s="7">
+        <v>0.9446</v>
+      </c>
+    </row>
+    <row r="27" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C27" s="3">
+        <v>0.51380000000000003</v>
+      </c>
+      <c r="D27" s="6">
+        <v>0.55210000000000004</v>
+      </c>
+      <c r="E27" s="7">
+        <v>0.53539999999999999</v>
+      </c>
+      <c r="F27" s="6">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="G27" s="7">
+        <v>0.52139999999999997</v>
+      </c>
+      <c r="H27" s="6">
+        <v>0.4945</v>
+      </c>
+      <c r="I27" s="7">
+        <v>0.52729999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C28" s="4">
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="D28" s="6">
+        <v>0.55559999999999998</v>
+      </c>
+      <c r="E28" s="7">
+        <v>0.56889999999999996</v>
+      </c>
+      <c r="F28" s="6">
+        <v>0.5514</v>
+      </c>
+      <c r="G28" s="7">
+        <v>0.53520000000000001</v>
+      </c>
+      <c r="H28" s="6">
+        <v>0.60750000000000004</v>
+      </c>
+      <c r="I28" s="7">
+        <v>0.58620000000000005</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F36F9018-B19D-4C41-8C32-7CC9583DDCF8}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding frame differencing and baseline code
</commit_message>
<xml_diff>
--- a/ExperimentList.xlsx
+++ b/ExperimentList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://herts365-my.sharepoint.com/personal/bt22aak_herts_ac_uk/Documents/ProjectWorkables/MscProjectRepo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="8_{8FB7EE8C-03D5-490C-A022-36A164B0F0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C1644EB-2B43-4BDF-844C-135854DA1F06}"/>
+  <xr:revisionPtr revIDLastSave="112" documentId="8_{8FB7EE8C-03D5-490C-A022-36A164B0F0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A65D4A2F-9B0B-461C-86E9-9CF074A52D65}"/>
   <bookViews>
-    <workbookView xWindow="69" yWindow="17" windowWidth="16388" windowHeight="8726" activeTab="2" xr2:uid="{373AC7B1-6464-4577-8099-CCADA7A31CED}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{373AC7B1-6464-4577-8099-CCADA7A31CED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Exp Name</t>
   </si>
@@ -107,13 +107,40 @@
   </si>
   <si>
     <t>Exp_2_7_Canny_125_250</t>
+  </si>
+  <si>
+    <t>Exp_5_1_FrameDiff</t>
+  </si>
+  <si>
+    <t>Exp_10_1_contour_OF</t>
+  </si>
+  <si>
+    <t>The method involves frame differencing</t>
+  </si>
+  <si>
+    <t>Combinataion of contour deteciton an optical flow</t>
+  </si>
+  <si>
+    <t>Exp_6_1_Baseline</t>
+  </si>
+  <si>
+    <t>Base line with no transformation. Raw resized Image</t>
+  </si>
+  <si>
+    <t>Using a Different edge detectors in combination with Background subtraction using MOG2 method</t>
+  </si>
+  <si>
+    <t>Using canny edge detectors, the parameters where changed to identify its impact</t>
+  </si>
+  <si>
+    <t>Using canny edge detector in combination with mog2 BG subtraction, different resolutions were compared.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,19 +168,35 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -173,8 +216,19 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -256,42 +310,83 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="20% - Accent4" xfId="2" builtinId="42"/>
+    <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -305,10 +400,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -628,149 +719,258 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B813C3E1-A61A-440A-8F3C-00DD70075391}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.07421875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.07421875" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.4609375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.3828125" customWidth="1"/>
+    <col min="3" max="3" width="43" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.23046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
+      <c r="A1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="12" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B2" t="s">
+      <c r="A2" s="14">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>10</v>
       </c>
+      <c r="C2" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B3" t="s">
+      <c r="A3" s="14"/>
+      <c r="B3" s="15" t="s">
         <v>11</v>
       </c>
+      <c r="C3" s="16"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B4" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="15" t="s">
         <v>12</v>
       </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B5" t="s">
+      <c r="A5" s="14"/>
+      <c r="B5" s="15" t="s">
         <v>13</v>
       </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B6" t="s">
+      <c r="A6" s="14"/>
+      <c r="B6" s="15" t="s">
         <v>14</v>
       </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B7" t="s">
+      <c r="A7" s="14"/>
+      <c r="B7" s="15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A8" s="14">
+        <v>2</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+    </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A9" s="10">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
+      <c r="A9" s="14"/>
+      <c r="B9" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A10" s="10"/>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
+      <c r="A10" s="14"/>
+      <c r="B10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A11" s="10"/>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
+      <c r="A11" s="14"/>
+      <c r="B11" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A12" s="10"/>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
+      <c r="A12" s="14"/>
+      <c r="B12" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A13" s="10"/>
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
+      <c r="A13" s="14"/>
+      <c r="B13" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A14" s="10"/>
-      <c r="B14" t="s">
-        <v>21</v>
-      </c>
+      <c r="A14" s="14"/>
+      <c r="B14" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A15" s="10"/>
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A17" s="10">
+      <c r="A15" s="14">
         <v>3</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B15" s="15" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A18" s="10"/>
-      <c r="B18" t="s">
+      <c r="C15" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A16" s="14"/>
+      <c r="B16" s="15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A19" s="10"/>
-      <c r="B19" t="s">
+      <c r="C16" s="16"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A17" s="14"/>
+      <c r="B17" s="15" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A20" s="10"/>
-      <c r="B20" t="s">
+      <c r="C17" s="16"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A18" s="14"/>
+      <c r="B18" s="15" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A21" s="10"/>
-      <c r="B21" t="s">
+      <c r="C18" s="16"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A19" s="14"/>
+      <c r="B19" s="15" t="s">
         <v>9</v>
       </c>
+      <c r="C19" s="16"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A20" s="17">
+        <v>4</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A21" s="17">
+        <v>5</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A22" s="17">
+        <v>6</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A9:A15"/>
+  <mergeCells count="6">
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="C2:C7"/>
+    <mergeCell ref="C8:C14"/>
+    <mergeCell ref="A2:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -787,646 +987,646 @@
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="2">
+      <c r="A1" s="1">
         <v>1883</v>
       </c>
-      <c r="B1" s="3">
+      <c r="B1" s="2">
         <v>57580</v>
       </c>
-      <c r="C1" s="3">
+      <c r="C1" s="2">
         <v>3136</v>
       </c>
-      <c r="D1" s="4">
+      <c r="D1" s="3">
         <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>1891</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>58026</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>2690</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>1890</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>57952</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>2764</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>1888</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>57735</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>2981</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="8">
+      <c r="A5" s="7">
         <v>1900</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>57635</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>3081</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <v>1883</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <v>1891</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="4">
         <v>1890</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="4">
         <v>1888</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="7">
         <v>1900</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <v>57580</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <v>58026</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="6">
         <v>57952</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="5">
         <v>57735</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="6">
         <v>57635</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <v>3136</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="5">
         <v>2690</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="6">
         <v>2764</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="5">
         <v>2981</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="6">
         <v>3081</v>
       </c>
-      <c r="P8" s="9">
+      <c r="P8" s="8">
         <v>0.94499999999999995</v>
       </c>
-      <c r="Q8" s="3">
+      <c r="Q8" s="2">
         <v>0.35639999999999999</v>
       </c>
-      <c r="R8" s="3">
+      <c r="R8" s="2">
         <v>0.98850000000000005</v>
       </c>
-      <c r="S8" s="3">
+      <c r="S8" s="2">
         <v>0.94369999999999998</v>
       </c>
-      <c r="T8" s="3">
+      <c r="T8" s="2">
         <v>0.52929999999999999</v>
       </c>
-      <c r="U8" s="4">
+      <c r="U8" s="3">
         <v>0.57720000000000005</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>33</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <v>25</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="6">
         <v>26</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="5">
         <v>28</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="6">
         <v>16</v>
       </c>
-      <c r="P9" s="5">
+      <c r="P9" s="4">
         <v>0.91539999999999999</v>
       </c>
-      <c r="Q9" s="6">
+      <c r="Q9" s="5">
         <v>0.26290000000000002</v>
       </c>
-      <c r="R9" s="6">
+      <c r="R9" s="5">
         <v>0.97809999999999997</v>
       </c>
-      <c r="S9" s="6">
+      <c r="S9" s="5">
         <v>0.91349999999999998</v>
       </c>
-      <c r="T9" s="6">
+      <c r="T9" s="5">
         <v>0.41439999999999999</v>
       </c>
-      <c r="U9" s="6">
+      <c r="U9" s="5">
         <v>0.93569999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="P10" s="5">
+      <c r="P10" s="4">
         <v>0.95430000000000004</v>
       </c>
-      <c r="Q10" s="7">
+      <c r="Q10" s="6">
         <v>0.39989999999999998</v>
       </c>
-      <c r="R10" s="7">
+      <c r="R10" s="6">
         <v>0.98540000000000005</v>
       </c>
-      <c r="S10" s="7">
+      <c r="S10" s="6">
         <v>0.95330000000000004</v>
       </c>
-      <c r="T10" s="7">
+      <c r="T10" s="6">
         <v>0.56889999999999996</v>
       </c>
-      <c r="U10" s="7">
+      <c r="U10" s="6">
         <v>0.48370000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="P11" s="5">
+      <c r="P11" s="4">
         <v>0.94589999999999996</v>
       </c>
-      <c r="Q11" s="6">
+      <c r="Q11" s="5">
         <v>0.36</v>
       </c>
-      <c r="R11" s="6">
+      <c r="R11" s="5">
         <v>0.98880000000000001</v>
       </c>
-      <c r="S11" s="6">
+      <c r="S11" s="5">
         <v>0.9446</v>
       </c>
-      <c r="T11" s="6">
+      <c r="T11" s="5">
         <v>0.52769999999999995</v>
       </c>
-      <c r="U11" s="6">
+      <c r="U11" s="5">
         <v>0.61580000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="P12" s="5">
+      <c r="P12" s="4">
         <v>0.94320000000000004</v>
       </c>
-      <c r="Q12" s="7">
+      <c r="Q12" s="6">
         <v>0.34849999999999998</v>
       </c>
-      <c r="R12" s="7">
+      <c r="R12" s="6">
         <v>0.98429999999999995</v>
       </c>
-      <c r="S12" s="7">
+      <c r="S12" s="6">
         <v>0.94189999999999996</v>
       </c>
-      <c r="T12" s="7">
+      <c r="T12" s="6">
         <v>0.51470000000000005</v>
       </c>
-      <c r="U12" s="7">
+      <c r="U12" s="6">
         <v>0.84870000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="P13" s="8">
+      <c r="P13" s="7">
         <v>0.94189999999999996</v>
       </c>
-      <c r="Q13" s="6">
+      <c r="Q13" s="5">
         <v>0.3427</v>
       </c>
-      <c r="R13" s="6">
+      <c r="R13" s="5">
         <v>0.98119999999999996</v>
       </c>
-      <c r="S13" s="6">
+      <c r="S13" s="5">
         <v>0.94059999999999999</v>
       </c>
-      <c r="T13" s="6">
+      <c r="T13" s="5">
         <v>0.50800000000000001</v>
       </c>
-      <c r="U13" s="6">
+      <c r="U13" s="5">
         <v>0.63270000000000004</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C14" s="9">
+      <c r="C14" s="8">
         <v>0.94499999999999995</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>0.91539999999999999</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <v>0.95430000000000004</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="4">
         <v>0.94589999999999996</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="4">
         <v>0.94320000000000004</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="7">
         <v>0.94189999999999996</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>0.35639999999999999</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <v>0.26290000000000002</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="6">
         <v>0.39989999999999998</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="5">
         <v>0.36</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="6">
         <v>0.34849999999999998</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="5">
         <v>0.3427</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <v>0.98850000000000005</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="5">
         <v>0.97809999999999997</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="6">
         <v>0.98540000000000005</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="5">
         <v>0.98880000000000001</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="6">
         <v>0.98429999999999995</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="5">
         <v>0.98119999999999996</v>
       </c>
     </row>
     <row r="17" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>0.94369999999999998</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="5">
         <v>0.91349999999999998</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <v>0.95330000000000004</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="5">
         <v>0.9446</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="6">
         <v>0.94189999999999996</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="5">
         <v>0.94059999999999999</v>
       </c>
     </row>
     <row r="18" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>0.52929999999999999</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="5">
         <v>0.41439999999999999</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="6">
         <v>0.56889999999999996</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="5">
         <v>0.52769999999999995</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="6">
         <v>0.51470000000000005</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="5">
         <v>0.50800000000000001</v>
       </c>
     </row>
     <row r="19" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C19" s="4">
+      <c r="C19" s="3">
         <v>0.57720000000000005</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="5">
         <v>0.93569999999999998</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="6">
         <v>0.48370000000000002</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="5">
         <v>0.61580000000000001</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="6">
         <v>0.84870000000000001</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="5">
         <v>0.63270000000000004</v>
       </c>
-      <c r="L19" s="9">
+      <c r="L19" s="8">
         <v>0.94269999999999998</v>
       </c>
-      <c r="M19" s="3">
+      <c r="M19" s="2">
         <v>0.34699999999999998</v>
       </c>
-      <c r="N19" s="3">
+      <c r="N19" s="2">
         <v>0.98899999999999999</v>
       </c>
-      <c r="O19" s="3">
+      <c r="O19" s="2">
         <v>0.94130000000000003</v>
       </c>
-      <c r="P19" s="3">
+      <c r="P19" s="2">
         <v>0.51380000000000003</v>
       </c>
-      <c r="Q19" s="4">
+      <c r="Q19" s="3">
         <v>0.52300000000000002</v>
       </c>
     </row>
     <row r="20" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="L20" s="5">
+      <c r="L20" s="4">
         <v>0.95089999999999997</v>
       </c>
-      <c r="M20" s="6">
+      <c r="M20" s="5">
         <v>0.38290000000000002</v>
       </c>
-      <c r="N20" s="6">
+      <c r="N20" s="5">
         <v>0.98899999999999999</v>
       </c>
-      <c r="O20" s="6">
+      <c r="O20" s="5">
         <v>0.94969999999999999</v>
       </c>
-      <c r="P20" s="6">
+      <c r="P20" s="5">
         <v>0.55210000000000004</v>
       </c>
-      <c r="Q20" s="6">
+      <c r="Q20" s="5">
         <v>0.55559999999999998</v>
       </c>
     </row>
     <row r="21" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="L21" s="5">
+      <c r="L21" s="4">
         <v>0.94769999999999999</v>
       </c>
-      <c r="M21" s="7">
+      <c r="M21" s="6">
         <v>0.36759999999999998</v>
       </c>
-      <c r="N21" s="7">
+      <c r="N21" s="6">
         <v>0.9849</v>
       </c>
-      <c r="O21" s="7">
+      <c r="O21" s="6">
         <v>0.94650000000000001</v>
       </c>
-      <c r="P21" s="7">
+      <c r="P21" s="6">
         <v>0.53539999999999999</v>
       </c>
-      <c r="Q21" s="7">
+      <c r="Q21" s="6">
         <v>0.56889999999999996</v>
       </c>
     </row>
     <row r="22" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="L22" s="5">
+      <c r="L22" s="4">
         <v>0.95420000000000005</v>
       </c>
-      <c r="M22" s="6">
+      <c r="M22" s="5">
         <v>0.39939999999999998</v>
       </c>
-      <c r="N22" s="6">
+      <c r="N22" s="5">
         <v>0.98640000000000005</v>
       </c>
-      <c r="O22" s="6">
+      <c r="O22" s="5">
         <v>0.95320000000000005</v>
       </c>
-      <c r="P22" s="6">
+      <c r="P22" s="5">
         <v>0.56799999999999995</v>
       </c>
-      <c r="Q22" s="6">
+      <c r="Q22" s="5">
         <v>0.5514</v>
       </c>
     </row>
     <row r="23" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C23" s="9">
+      <c r="C23" s="8">
         <v>0.94269999999999998</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="4">
         <v>0.95089999999999997</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="4">
         <v>0.94769999999999999</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="4">
         <v>0.95420000000000005</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G23" s="4">
         <v>0.94440000000000002</v>
       </c>
-      <c r="H23" s="5">
+      <c r="H23" s="4">
         <v>0.93810000000000004</v>
       </c>
-      <c r="I23" s="8">
+      <c r="I23" s="7">
         <v>0.94589999999999996</v>
       </c>
-      <c r="L23" s="5">
+      <c r="L23" s="4">
         <v>0.94440000000000002</v>
       </c>
-      <c r="M23" s="7">
+      <c r="M23" s="6">
         <v>0.35399000000000003</v>
       </c>
-      <c r="N23" s="7">
+      <c r="N23" s="6">
         <v>0.99009999999999998</v>
       </c>
-      <c r="O23" s="7">
+      <c r="O23" s="6">
         <v>0.94289999999999996</v>
       </c>
-      <c r="P23" s="7">
+      <c r="P23" s="6">
         <v>0.52139999999999997</v>
       </c>
-      <c r="Q23" s="7">
+      <c r="Q23" s="6">
         <v>0.53520000000000001</v>
       </c>
     </row>
     <row r="24" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <v>0.34699999999999998</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="5">
         <v>0.38290000000000002</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="6">
         <v>0.36759999999999998</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="5">
         <v>0.39939999999999998</v>
       </c>
-      <c r="G24" s="7">
+      <c r="G24" s="6">
         <v>0.35399000000000003</v>
       </c>
-      <c r="H24" s="6">
+      <c r="H24" s="5">
         <v>0.32969999999999999</v>
       </c>
-      <c r="I24" s="7">
+      <c r="I24" s="6">
         <v>0.3599</v>
       </c>
-      <c r="L24" s="5">
+      <c r="L24" s="4">
         <v>0.93810000000000004</v>
       </c>
-      <c r="M24" s="6">
+      <c r="M24" s="5">
         <v>0.32969999999999999</v>
       </c>
-      <c r="N24" s="6">
+      <c r="N24" s="5">
         <v>0.98899999999999999</v>
       </c>
-      <c r="O24" s="6">
+      <c r="O24" s="5">
         <v>0.9365</v>
       </c>
-      <c r="P24" s="6">
+      <c r="P24" s="5">
         <v>0.4945</v>
       </c>
-      <c r="Q24" s="6">
+      <c r="Q24" s="5">
         <v>0.60750000000000004</v>
       </c>
     </row>
     <row r="25" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C25" s="3">
+      <c r="C25" s="2">
         <v>0.98899999999999999</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="5">
         <v>0.98899999999999999</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="6">
         <v>0.9849</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="5">
         <v>0.98640000000000005</v>
       </c>
-      <c r="G25" s="7">
+      <c r="G25" s="6">
         <v>0.99009999999999998</v>
       </c>
-      <c r="H25" s="6">
+      <c r="H25" s="5">
         <v>0.98899999999999999</v>
       </c>
-      <c r="I25" s="7">
+      <c r="I25" s="6">
         <v>0.98640000000000005</v>
       </c>
-      <c r="L25" s="8">
+      <c r="L25" s="7">
         <v>0.94589999999999996</v>
       </c>
-      <c r="M25" s="7">
+      <c r="M25" s="6">
         <v>0.3599</v>
       </c>
-      <c r="N25" s="7">
+      <c r="N25" s="6">
         <v>0.98640000000000005</v>
       </c>
-      <c r="O25" s="7">
+      <c r="O25" s="6">
         <v>0.9446</v>
       </c>
-      <c r="P25" s="7">
+      <c r="P25" s="6">
         <v>0.52729999999999999</v>
       </c>
-      <c r="Q25" s="7">
+      <c r="Q25" s="6">
         <v>0.58620000000000005</v>
       </c>
     </row>
     <row r="26" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C26" s="3">
+      <c r="C26" s="2">
         <v>0.94130000000000003</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="5">
         <v>0.94969999999999999</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="6">
         <v>0.94650000000000001</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="5">
         <v>0.95320000000000005</v>
       </c>
-      <c r="G26" s="7">
+      <c r="G26" s="6">
         <v>0.94289999999999996</v>
       </c>
-      <c r="H26" s="6">
+      <c r="H26" s="5">
         <v>0.9365</v>
       </c>
-      <c r="I26" s="7">
+      <c r="I26" s="6">
         <v>0.9446</v>
       </c>
     </row>
     <row r="27" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C27" s="3">
+      <c r="C27" s="2">
         <v>0.51380000000000003</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="5">
         <v>0.55210000000000004</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="6">
         <v>0.53539999999999999</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27" s="5">
         <v>0.56799999999999995</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G27" s="6">
         <v>0.52139999999999997</v>
       </c>
-      <c r="H27" s="6">
+      <c r="H27" s="5">
         <v>0.4945</v>
       </c>
-      <c r="I27" s="7">
+      <c r="I27" s="6">
         <v>0.52729999999999999</v>
       </c>
     </row>
     <row r="28" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C28" s="4">
+      <c r="C28" s="3">
         <v>0.52300000000000002</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="5">
         <v>0.55559999999999998</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="6">
         <v>0.56889999999999996</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F28" s="5">
         <v>0.5514</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G28" s="6">
         <v>0.53520000000000001</v>
       </c>
-      <c r="H28" s="6">
+      <c r="H28" s="5">
         <v>0.60750000000000004</v>
       </c>
-      <c r="I28" s="7">
+      <c r="I28" s="6">
         <v>0.58620000000000005</v>
       </c>
     </row>
@@ -1439,7 +1639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F36F9018-B19D-4C41-8C32-7CC9583DDCF8}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData/>

</xml_diff>